<commit_message>
[feat][wip] added real-time traffic light modules
What: Added the real-time traffic light python module. IT WILL NOT RUN AS IS

Why: This module will be a good example going forward for controlling traffic lights via TRACI
</commit_message>
<xml_diff>
--- a/intersection_parameters/traffic_light_phasing.xlsx
+++ b/intersection_parameters/traffic_light_phasing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">traffic_light_id</t>
   </si>
@@ -34,43 +34,16 @@
     <t xml:space="preserve">key</t>
   </si>
   <si>
-    <t xml:space="preserve">grrrgrrgrrrgrr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">srrrrrrsrrrrrr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,6,6,6,1,8,3,2,2,2,2,5,4,7</t>
+    <t xml:space="preserve">srgsrrrsrgsrrr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srrsrrgsrrsrrg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,6,1,8,8,8,3,2,2,5,4,4,4,7</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">grrrrrrrrrgrrr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">srrrrrrrrrrrrr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,6,6,6,1,1,4,4,2,2,5,3,3,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rrrrgrrrrrrgsrr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">srrrrrrsrrrrrrr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,6,6,6,1,4,7,2,2,2,2,5,8,8,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rrrrrgrr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rrrrrrrr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,6,6,2,2,5,4,4</t>
   </si>
 </sst>
 </file>
@@ -171,16 +144,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.94"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
@@ -214,48 +188,6 @@
       </c>
       <c r="F2" s="0" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>63069007</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>63069008</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>63069009</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>